<commit_message>
Add Revisi Test Case Search and Rating
</commit_message>
<xml_diff>
--- a/test_case/Test Case Search dan Rating.xlsx
+++ b/test_case/Test Case Search dan Rating.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UPI\Semester 1\Semester 1\PRPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4301F8B-D798-4BFD-AF66-D75E4A326AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4342D5AC-FA63-4A95-B484-A491CD587F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{7A22DF56-4116-4A57-A550-1282D1AD0C43}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{7A22DF56-4116-4A57-A550-1282D1AD0C43}"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
-    <sheet name="Rating Users" sheetId="2" r:id="rId2"/>
+    <sheet name="Rating Users &amp;Admin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="213">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -58,31 +58,16 @@
 Case ID</t>
   </si>
   <si>
-    <t>TC01</t>
-  </si>
-  <si>
     <t>Search berdasarkan 
 nama pengelola 
 dengan data valid</t>
   </si>
   <si>
-    <t>TC02</t>
-  </si>
-  <si>
     <t>Search berdasarkan 
 nama bank sampah
 dengan data valid</t>
   </si>
   <si>
-    <t>TC03</t>
-  </si>
-  <si>
-    <t>TC04</t>
-  </si>
-  <si>
-    <t>TC05</t>
-  </si>
-  <si>
     <t>Search berdasarkan 
 harga sampah organik dengan data valid</t>
   </si>
@@ -112,21 +97,6 @@
     <t>Search berdasarkan 
 harga sampah 
 non organik dengan data valid</t>
-  </si>
-  <si>
-    <t>TC06</t>
-  </si>
-  <si>
-    <t>TC07</t>
-  </si>
-  <si>
-    <t>TC08</t>
-  </si>
-  <si>
-    <t>TC09</t>
-  </si>
-  <si>
-    <t>TC10</t>
   </si>
   <si>
     <t>Search berdasarkan 
@@ -232,51 +202,6 @@
 harga sampah non organik dengan input simbol</t>
   </si>
   <si>
-    <t>TC11</t>
-  </si>
-  <si>
-    <t>TC12</t>
-  </si>
-  <si>
-    <t>TC13</t>
-  </si>
-  <si>
-    <t>TC14</t>
-  </si>
-  <si>
-    <t>TC16</t>
-  </si>
-  <si>
-    <t>TC17</t>
-  </si>
-  <si>
-    <t>TC18</t>
-  </si>
-  <si>
-    <t>TC19</t>
-  </si>
-  <si>
-    <t>TC20</t>
-  </si>
-  <si>
-    <t>TC21</t>
-  </si>
-  <si>
-    <t>TC22</t>
-  </si>
-  <si>
-    <t>TC23</t>
-  </si>
-  <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
-    <t>TC26</t>
-  </si>
-  <si>
     <t>Search dengan tipe data 
 string pada bagian 
 kategori</t>
@@ -302,24 +227,6 @@
   <si>
     <t>Search berdasarkan 
 lokasi dengan angka</t>
-  </si>
-  <si>
-    <t>TC27</t>
-  </si>
-  <si>
-    <t>TC28</t>
-  </si>
-  <si>
-    <t>TC29</t>
-  </si>
-  <si>
-    <t>TC30</t>
-  </si>
-  <si>
-    <t>TC31</t>
-  </si>
-  <si>
-    <t>TC32</t>
   </si>
   <si>
     <t>Search berdasarkan 
@@ -452,9 +359,6 @@
     <t>Nama Bank Sampah:</t>
   </si>
   <si>
-    <t>Nama Pengelola</t>
-  </si>
-  <si>
     <t>Lokasi:</t>
   </si>
   <si>
@@ -462,13 +366,6 @@
   </si>
   <si>
     <t xml:space="preserve">Harga Sampah NOn Organik: </t>
-  </si>
-  <si>
-    <t>Lokasi: @!&amp;$#</t>
-  </si>
-  <si>
-    <t>Harga Sampah 
-Non Organik: @!&amp;$#</t>
   </si>
   <si>
     <t>Kategori: Nama</t>
@@ -529,9 +426,6 @@
     <t>Memberikan rating untuk bank sampah dengan simbol</t>
   </si>
   <si>
-    <t>Memilih ID bank sampah dengan data valid</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Jalankan Program
 2. Ketik 4 (Rating Bank Sampah)
 3. Pilih bank sampah
@@ -539,21 +433,6 @@
 </t>
   </si>
   <si>
-    <t>ID Bank sampah: 1</t>
-  </si>
-  <si>
-    <t>ID Bank sampah: 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Bank Sampah: </t>
-  </si>
-  <si>
-    <t>ID Bank Sampah: Satu</t>
-  </si>
-  <si>
-    <t>ID Bank Sampah: !$%</t>
-  </si>
-  <si>
     <t>Rating: 5</t>
   </si>
   <si>
@@ -578,16 +457,6 @@
 4. Klik enter</t>
   </si>
   <si>
-    <t>Data rating sebelumnya
-sudah tersimpan, sehingga tidak dapat memberikan rating kembali</t>
-  </si>
-  <si>
-    <t>Menampilkan perintah untuk memberikan rating</t>
-  </si>
-  <si>
-    <t>Menampilkan message error</t>
-  </si>
-  <si>
     <t>Menampilkan detail 
 bank sampah dengan nama "Sumera TrashBank"</t>
   </si>
@@ -595,12 +464,6 @@
     <t>Sistem menampilkan pesan "Tidak ada hasil yang mendekati nama bank sampah tersebut"</t>
   </si>
   <si>
-    <t>Sistem menampilkan pesan 
-"Tidak ada hasil yang 
-mendekati nama bank 
-sampah tersebut"</t>
-  </si>
-  <si>
     <t>Menampilkan detail 
 bank sampah dengan nama pengelola "Jakiii"</t>
   </si>
@@ -618,16 +481,6 @@
     <t>Sistem menampilkan pesan "Tidak ada hasil yang mendekati harga sampah tersebut"</t>
   </si>
   <si>
-    <t>Menampilkan nama bank 
-sampah yang relevan dengan kata kunci</t>
-  </si>
-  <si>
-    <t>Menampilkan nama pengelola yang relevan dengan kata kunci</t>
-  </si>
-  <si>
-    <t>Menampilkan lokasi yang relevan dengan kata kunci</t>
-  </si>
-  <si>
     <t>Menampilkan harga 
 sampah yang relevan dengan kata kunci</t>
   </si>
@@ -646,21 +499,6 @@
   <si>
     <t>1. Jalankan Program
 2. Ketik 3 (Search Bank Sampah)
-3. Ketik 1 (Nama Bank Sampah)
-4. Masukkan nama bank sampah
-5. Klik enter</t>
-  </si>
-  <si>
-    <t>Search berdasarkan 
-nama bank sampah 
-dengan data yang hampir mirip</t>
-  </si>
-  <si>
-    <t>Nama Bank Sampah: sumara</t>
-  </si>
-  <si>
-    <t>1. Jalankan Program
-2. Ketik 3 (Search Bank Sampah)
 3. Ketik 2 (Nama Pengelola Bank Sampah)
 4. Masukkan nama pengelola dengan kata kunci tidak lengkap
 5. Klik enter</t>
@@ -773,30 +611,7 @@
 5. Klik enter</t>
   </si>
   <si>
-    <t>Sistem menampilkan pesan 
-"Tidak ada hasil yang 
-mendekati harga sampah 
-tersebut"</t>
-  </si>
-  <si>
-    <t>Harga Sampah Organik: 
-@!&amp;$#</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nama Bank Sampah: 834 </t>
-  </si>
-  <si>
-    <t>Sistem menampilkan pesan 
-"Tidak ada hasil yang 
-mendekati harga sampah
- tersebut"</t>
-  </si>
-  <si>
-    <t>Menampilkan message 
-error</t>
-  </si>
-  <si>
-    <t>Memilih opsi bank sampah yang tidak terdaftar di data</t>
   </si>
   <si>
     <t>Membatalkan proses rating setelah memilih opsi rating bank sampah</t>
@@ -810,10 +625,294 @@
     <t>Kembali ke menu utama</t>
   </si>
   <si>
-    <t>TC15</t>
-  </si>
-  <si>
-    <t>TC33</t>
+    <t>Rating berhasil disimpan 
+dan menampilkan pesan 
+"Terima kasih telah 
+memberi penilaian untuk 
+[nama Bank Sampah]"</t>
+  </si>
+  <si>
+    <t>Menampilkan nama bank 
+sampah yang mendekati dengan kata kunci</t>
+  </si>
+  <si>
+    <t>Menampilkan nama pengelola yang mendekati dengan kata kunci</t>
+  </si>
+  <si>
+    <t>Menampilkan lokasi yang mendekati dengan kata kunci</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Silakan pilih kategori 
+berdasarkan angka yang 
+tersedia"</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Input pencarian tidak 
+boleh kosong!"</t>
+  </si>
+  <si>
+    <t>Nama Pengelola:</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Input pencarian tidak 
+boleh kosong"</t>
+  </si>
+  <si>
+    <t>Menampilkan pesan 
+"Silakan pilih kategori 
+berdasarkan angka yang 
+tersedia"</t>
+  </si>
+  <si>
+    <t>Menampilkan pesan 
+"Tidak ada hasil yang 
+mendekati nama bank sampah tersebut"</t>
+  </si>
+  <si>
+    <t>Menampilkan pesan 
+"Tidak ada hasil yang 
+mendekati lokasi bank sampah tersebut"</t>
+  </si>
+  <si>
+    <t>Menampilkan pesan 
+"Tidak ada hasil yang 
+mendekati nama pengelola bank sampah tersebut"</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Pencarian harga organik 
+hanya boleh mengirim 
+angka saja!"</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Pencarian harga non organik 
+hanya boleh mengirim 
+angka saja!"</t>
+  </si>
+  <si>
+    <t>Harga Sampah 
+Non Organik: @!&amp;$</t>
+  </si>
+  <si>
+    <t>Harga Sampah Organik: 
+@!&amp;$</t>
+  </si>
+  <si>
+    <t>Lokasi: @!&amp;$</t>
+  </si>
+  <si>
+    <t>Menampilkan peingatan 
+"Silakan pilih kategori 
+berdasarkan angka yang 
+tersedia"</t>
+  </si>
+  <si>
+    <t>Sistem menampilkan pesan "Tidak ada hasil yang mendekati nama pengelola bank sampah tersebut"</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Pencarian harga organik 
+hanya boleh menginputkan angka saja"</t>
+  </si>
+  <si>
+    <t>Menampilkan peringatan 
+"Pencarian harga non organik 
+hanya boleh menginputkan angka saja"</t>
+  </si>
+  <si>
+    <t>SC01</t>
+  </si>
+  <si>
+    <t>SC02</t>
+  </si>
+  <si>
+    <t>SC03</t>
+  </si>
+  <si>
+    <t>SC04</t>
+  </si>
+  <si>
+    <t>SC05</t>
+  </si>
+  <si>
+    <t>SC06</t>
+  </si>
+  <si>
+    <t>SC07</t>
+  </si>
+  <si>
+    <t>SC08</t>
+  </si>
+  <si>
+    <t>SC09</t>
+  </si>
+  <si>
+    <t>SC10</t>
+  </si>
+  <si>
+    <t>SC11</t>
+  </si>
+  <si>
+    <t>SC12</t>
+  </si>
+  <si>
+    <t>SC13</t>
+  </si>
+  <si>
+    <t>SC14</t>
+  </si>
+  <si>
+    <t>SC15</t>
+  </si>
+  <si>
+    <t>SC16</t>
+  </si>
+  <si>
+    <t>SC17</t>
+  </si>
+  <si>
+    <t>SC18</t>
+  </si>
+  <si>
+    <t>SC19</t>
+  </si>
+  <si>
+    <t>SC20</t>
+  </si>
+  <si>
+    <t>SC21</t>
+  </si>
+  <si>
+    <t>SC22</t>
+  </si>
+  <si>
+    <t>SC23</t>
+  </si>
+  <si>
+    <t>SC24</t>
+  </si>
+  <si>
+    <t>SC25</t>
+  </si>
+  <si>
+    <t>SC26</t>
+  </si>
+  <si>
+    <t>SC27</t>
+  </si>
+  <si>
+    <t>SC28</t>
+  </si>
+  <si>
+    <t>SC29</t>
+  </si>
+  <si>
+    <t>SC30</t>
+  </si>
+  <si>
+    <t>SC31</t>
+  </si>
+  <si>
+    <t>SC32</t>
+  </si>
+  <si>
+    <t>Memilih nomor bank sampah dengan data valid</t>
+  </si>
+  <si>
+    <t>No Bank sampah: 1</t>
+  </si>
+  <si>
+    <t>No Bank sampah: 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Bank Sampah: </t>
+  </si>
+  <si>
+    <t>No Bank Sampah: Satu</t>
+  </si>
+  <si>
+    <t>Memilih nomor bank sampah yang tidak terdaftar di data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menampilkan perintah untuk memberikan rating "Silakan pilih nomor bank sampah yang ingin diberi rating" </t>
+  </si>
+  <si>
+    <t>Menampilkan perintah "Silakan pilih opsi yang tersedia" dan dan menampilkan kembali data sampah yang tersedia</t>
+  </si>
+  <si>
+    <t>Menampilkan perintah "Silakan isi berdasarkan angka, hanya boleh berisi 1 angka" dan menampilkan kembali data sampah yang tersedia</t>
+  </si>
+  <si>
+    <t>No Bank Sampah: 1
+Rating: 5</t>
+  </si>
+  <si>
+    <t>1. Jalankan Program
+2. Ketik 4 (Rating Bank Sampah)
+3. Pilih bank sampah
+4. Klik enter
+5. Masukkan rating
+6. Klik enter</t>
+  </si>
+  <si>
+    <t>Menampilkan perintah 
+"Silakan rating bank sampah dari 1 sampai 5"  dan menampilkan kembali data bank sampah</t>
+  </si>
+  <si>
+    <t>Data rating sebelumnya
+sudah tersimpan, sehingga tidak dapat memberikan rating kembali dan menampilkan pesan "Rating Anda untuk [nama bank sampah] adalah [rating]!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistem menampilkan pesan "Tidak ada hasil yang mendekati nama bank sampah tersebut" </t>
+  </si>
+  <si>
+    <t>RT13</t>
+  </si>
+  <si>
+    <t>Membatalkan proses setelah memilih bank sampah yang akan diberikan rating</t>
+  </si>
+  <si>
+    <t>No Bank Sampah: !$%</t>
+  </si>
+  <si>
+    <t>RT01</t>
+  </si>
+  <si>
+    <t>RT02</t>
+  </si>
+  <si>
+    <t>RT03</t>
+  </si>
+  <si>
+    <t>RT04</t>
+  </si>
+  <si>
+    <t>RT05</t>
+  </si>
+  <si>
+    <t>RT06</t>
+  </si>
+  <si>
+    <t>RT07</t>
+  </si>
+  <si>
+    <t>RT08</t>
+  </si>
+  <si>
+    <t>RT09</t>
+  </si>
+  <si>
+    <t>RT10</t>
+  </si>
+  <si>
+    <t>RT11</t>
+  </si>
+  <si>
+    <t>RT12</t>
   </si>
 </sst>
 </file>
@@ -896,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -914,12 +1013,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -936,14 +1040,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0BF6B-DCD1-41C2-B786-EA00C08CA57A}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="B30" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1291,668 +1389,668 @@
     <col min="2" max="2" width="19.36328125" customWidth="1"/>
     <col min="3" max="3" width="26.6328125" customWidth="1"/>
     <col min="4" max="4" width="24.36328125" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>113</v>
+      <c r="G1" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>154</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>85</v>
+        <v>49</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>87</v>
+        <v>48</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>88</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>157</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>89</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>158</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>91</v>
+        <v>27</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>90</v>
+        <v>28</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>161</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>95</v>
+        <v>47</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>96</v>
+        <v>110</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>97</v>
+        <v>111</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>153</v>
+        <v>113</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>140</v>
+        <v>43</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="15"/>
+        <v>46</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="15"/>
+        <v>114</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="15"/>
+        <v>115</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="15"/>
+        <v>116</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="15"/>
+        <v>117</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>140</v>
+        <v>118</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>155</v>
+        <v>45</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E26" s="15"/>
+        <v>119</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>58</v>
+        <v>175</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="15"/>
+        <v>120</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>176</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E28" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="15"/>
+        <v>145</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>140</v>
+        <v>44</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>179</v>
+        <v>52</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>69</v>
+        <v>180</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>109</v>
+        <v>124</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>177</v>
+        <v>103</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>71</v>
+        <v>182</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>140</v>
+        <v>76</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>140</v>
+        <v>77</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1970,16 +2068,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96362DFF-2BFF-4E81-87A1-9FD3DD918FDF}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="2" max="2" width="22" style="16" customWidth="1"/>
     <col min="3" max="3" width="26.90625" customWidth="1"/>
     <col min="4" max="4" width="18.08984375" customWidth="1"/>
     <col min="5" max="5" width="20.6328125" customWidth="1"/>
@@ -1987,254 +2085,283 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>113</v>
+      <c r="G1" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>125</v>
+      <c r="A3" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>125</v>
+        <v>185</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>125</v>
+        <v>186</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>114</v>
+        <v>187</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>114</v>
+        <v>188</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+        <v>200</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>206</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="16"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>116</v>
+        <v>207</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>195</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>117</v>
+        <v>208</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>133</v>
+        <v>80</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>119</v>
+        <v>209</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>138</v>
+        <v>97</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>196</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>210</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" s="16"/>
+        <v>80</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>195</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>123</v>
+        <v>211</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E13" s="16"/>
+        <v>80</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>195</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>183</v>
+        <v>212</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>185</v>
+        <v>129</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>